<commit_message>
buscar comprobante en consulta cliente
</commit_message>
<xml_diff>
--- a/intranet/reportes/10180909350-202204.xlsx
+++ b/intranet/reportes/10180909350-202204.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>RUC</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>F001</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>00000000000</t>
   </si>
   <si>
     <t>**** DOCUMENTO ANULADO ****</t>
@@ -171,10 +177,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,7 +199,7 @@
     <col min="5" max="5" width="6"/>
     <col min="6" max="6" width="7"/>
     <col min="7" max="7" width="21"/>
-    <col min="8" max="8" width="10"/>
+    <col min="8" max="8" width="12"/>
     <col min="9" max="9" width="60"/>
     <col min="10" max="10" width="13"/>
     <col min="11" max="11" width="16"/>
@@ -305,19 +311,25 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s" s="3">
+        <v>25</v>
+      </c>
       <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M5" s="3">
+        <v>26</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M5" s="4">
         <v>0.00</v>
       </c>
       <c r="N5">
@@ -343,19 +355,25 @@
       <c r="F6">
         <v>2</v>
       </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>10329045159</v>
+      </c>
       <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="3">
+        <v>27</v>
+      </c>
+      <c r="J6" s="4">
         <v>17.80</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="4">
         <v>104.00</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="4">
         <v>3.20</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="4">
         <v>125.00</v>
       </c>
       <c r="N6">
@@ -373,27 +391,33 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M7" s="3">
+      <c r="J7" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M7" s="4">
         <v>0.00</v>
       </c>
       <c r="N7">
@@ -411,27 +435,33 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s" s="3">
+        <v>25</v>
+      </c>
       <c r="I8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M8" s="3">
+        <v>26</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M8" s="4">
         <v>0.00</v>
       </c>
       <c r="N8">
@@ -449,27 +479,33 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>46993209</v>
+      </c>
       <c r="I9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K9" s="3">
+        <v>30</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K9" s="4">
         <v>21.00</v>
       </c>
-      <c r="L9" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M9" s="3">
+      <c r="L9" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M9" s="4">
         <v>21.00</v>
       </c>
       <c r="N9">
@@ -487,27 +523,33 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>42993209</v>
+      </c>
       <c r="I10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K10" s="3">
+        <v>31</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K10" s="4">
         <v>12.00</v>
       </c>
-      <c r="L10" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="L10" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M10" s="4">
         <v>12.00</v>
       </c>
       <c r="N10">
@@ -525,27 +567,33 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>5</v>
       </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s" s="3">
+        <v>25</v>
+      </c>
       <c r="I11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M11" s="3">
+        <v>26</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M11" s="4">
         <v>0.00</v>
       </c>
       <c r="N11">
@@ -563,27 +611,33 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F12">
         <v>6</v>
       </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>71531120</v>
+      </c>
       <c r="I12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K12" s="3">
+        <v>32</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K12" s="4">
         <v>93.00</v>
       </c>
-      <c r="L12" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M12" s="3">
+      <c r="L12" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M12" s="4">
         <v>93.00</v>
       </c>
       <c r="N12">
@@ -601,27 +655,33 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F13">
         <v>7</v>
       </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s" s="3">
+        <v>25</v>
+      </c>
       <c r="I13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M13" s="3">
+        <v>26</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M13" s="4">
         <v>0.00</v>
       </c>
       <c r="N13">
@@ -639,27 +699,33 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F14">
         <v>8</v>
       </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
       <c r="I14" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K14" s="3">
+        <v>33</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K14" s="4">
         <v>79.00</v>
       </c>
-      <c r="L14" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M14" s="3">
+      <c r="L14" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M14" s="4">
         <v>79.00</v>
       </c>
       <c r="N14">
@@ -677,27 +743,33 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F15">
         <v>9</v>
       </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s" s="3">
+        <v>25</v>
+      </c>
       <c r="I15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M15" s="3">
+        <v>26</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M15" s="4">
         <v>0.00</v>
       </c>
       <c r="N15">
@@ -715,27 +787,33 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F16">
         <v>10</v>
       </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
       <c r="I16" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K16" s="3">
+        <v>33</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K16" s="4">
         <v>16.50</v>
       </c>
-      <c r="L16" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M16" s="3">
+      <c r="L16" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M16" s="4">
         <v>16.50</v>
       </c>
       <c r="N16">
@@ -753,27 +831,33 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F17">
         <v>11</v>
       </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1">
+        <v>20538633021</v>
+      </c>
       <c r="I17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K17" s="3">
+        <v>34</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K17" s="4">
         <v>49.00</v>
       </c>
-      <c r="L17" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M17" s="3">
+      <c r="L17" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M17" s="4">
         <v>49.00</v>
       </c>
       <c r="N17">
@@ -791,27 +875,33 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F18">
         <v>12</v>
       </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1">
+        <v>20538633021</v>
+      </c>
       <c r="I18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K18" s="3">
+        <v>34</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K18" s="4">
         <v>20.04</v>
       </c>
-      <c r="L18" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M18" s="3">
+      <c r="L18" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M18" s="4">
         <v>20.04</v>
       </c>
       <c r="N18">
@@ -829,27 +919,33 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F19">
         <v>13</v>
       </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
       <c r="I19" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K19" s="3">
+        <v>33</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K19" s="4">
         <v>14.00</v>
       </c>
-      <c r="L19" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M19" s="3">
+      <c r="L19" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M19" s="4">
         <v>14.00</v>
       </c>
       <c r="N19">
@@ -867,27 +963,33 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F20">
         <v>14</v>
       </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
       <c r="I20" t="s">
-        <v>31</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K20" s="3">
+        <v>33</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K20" s="4">
         <v>14.00</v>
       </c>
-      <c r="L20" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M20" s="3">
+      <c r="L20" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M20" s="4">
         <v>14.00</v>
       </c>
       <c r="N20">
@@ -905,27 +1007,33 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F21">
         <v>15</v>
       </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" t="s" s="3">
+        <v>25</v>
+      </c>
       <c r="I21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L21" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M21" s="3">
+        <v>26</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M21" s="4">
         <v>0.00</v>
       </c>
       <c r="N21">
@@ -943,27 +1051,33 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F22">
         <v>16</v>
       </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
       <c r="I22" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K22" s="3">
+        <v>33</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K22" s="4">
         <v>190.00</v>
       </c>
-      <c r="L22" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M22" s="3">
+      <c r="L22" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M22" s="4">
         <v>190.00</v>
       </c>
       <c r="N22">
@@ -981,27 +1095,33 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F23">
         <v>17</v>
       </c>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" t="s" s="3">
+        <v>25</v>
+      </c>
       <c r="I23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K23" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L23" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M23" s="3">
+        <v>26</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M23" s="4">
         <v>0.00</v>
       </c>
       <c r="N23">
@@ -1019,27 +1139,33 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F24">
         <v>18</v>
       </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>71531120</v>
+      </c>
       <c r="I24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J24" s="3">
+        <v>32</v>
+      </c>
+      <c r="J24" s="4">
         <v>25.42</v>
       </c>
-      <c r="K24" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L24" s="3">
+      <c r="K24" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L24" s="4">
         <v>4.58</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24" s="4">
         <v>30.00</v>
       </c>
       <c r="N24">
@@ -1057,27 +1183,33 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F25">
         <v>19</v>
       </c>
+      <c r="G25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
       <c r="I25" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K25" s="3">
+        <v>33</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K25" s="4">
         <v>50.00</v>
       </c>
-      <c r="L25" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M25" s="3">
+      <c r="L25" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M25" s="4">
         <v>50.00</v>
       </c>
       <c r="N25">
@@ -1095,27 +1227,33 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F26">
         <v>20</v>
       </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>32827663</v>
+      </c>
       <c r="I26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J26" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K26" s="3">
+        <v>35</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K26" s="4">
         <v>50.00</v>
       </c>
-      <c r="L26" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M26" s="3">
+      <c r="L26" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M26" s="4">
         <v>50.00</v>
       </c>
       <c r="N26">
@@ -1133,27 +1271,33 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F27">
         <v>21</v>
       </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>32954826</v>
+      </c>
       <c r="I27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K27" s="3">
+        <v>36</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K27" s="4">
         <v>87.00</v>
       </c>
-      <c r="L27" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M27" s="3">
+      <c r="L27" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M27" s="4">
         <v>87.00</v>
       </c>
       <c r="N27">
@@ -1171,27 +1315,33 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F28">
         <v>22</v>
       </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
       <c r="I28" t="s">
-        <v>31</v>
-      </c>
-      <c r="J28" s="3">
+        <v>33</v>
+      </c>
+      <c r="J28" s="4">
         <v>8.47</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="4">
         <v>20.00</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="4">
         <v>1.53</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28" s="4">
         <v>30.00</v>
       </c>
       <c r="N28">
@@ -1209,27 +1359,33 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F29">
         <v>23</v>
       </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>76284255</v>
+      </c>
       <c r="I29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J29" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K29" s="3">
+        <v>37</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K29" s="4">
         <v>40.00</v>
       </c>
-      <c r="L29" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M29" s="3">
+      <c r="L29" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M29" s="4">
         <v>40.00</v>
       </c>
       <c r="N29">
@@ -1247,27 +1403,33 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F30">
         <v>24</v>
       </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30" s="1">
+        <v>20538633021</v>
+      </c>
       <c r="I30" t="s">
-        <v>32</v>
-      </c>
-      <c r="J30" s="3">
+        <v>34</v>
+      </c>
+      <c r="J30" s="4">
         <v>29.66</v>
       </c>
-      <c r="K30" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L30" s="3">
+      <c r="K30" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L30" s="4">
         <v>5.34</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M30" s="4">
         <v>35.00</v>
       </c>
       <c r="N30">
@@ -1285,27 +1447,33 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F31">
         <v>25</v>
       </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>48436463</v>
+      </c>
       <c r="I31" t="s">
-        <v>36</v>
-      </c>
-      <c r="J31" s="3">
+        <v>38</v>
+      </c>
+      <c r="J31" s="4">
         <v>162.71</v>
       </c>
-      <c r="K31" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L31" s="3">
+      <c r="K31" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L31" s="4">
         <v>29.29</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="4">
         <v>192.00</v>
       </c>
       <c r="N31">
@@ -1323,27 +1491,33 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F32">
         <v>26</v>
       </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>46125003</v>
+      </c>
       <c r="I32" t="s">
-        <v>37</v>
-      </c>
-      <c r="J32" s="3">
+        <v>39</v>
+      </c>
+      <c r="J32" s="4">
         <v>16.95</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="4">
         <v>120.00</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="4">
         <v>3.05</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="4">
         <v>140.00</v>
       </c>
       <c r="N32">
@@ -1361,27 +1535,33 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F33">
         <v>27</v>
       </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
+        <v>24</v>
+      </c>
       <c r="I33" t="s">
-        <v>31</v>
-      </c>
-      <c r="J33" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K33" s="3">
+        <v>33</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K33" s="4">
         <v>8.00</v>
       </c>
-      <c r="L33" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M33" s="3">
+      <c r="L33" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M33" s="4">
         <v>8.00</v>
       </c>
       <c r="N33">
@@ -1399,27 +1579,33 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F34">
         <v>28</v>
       </c>
+      <c r="G34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" t="s">
+        <v>24</v>
+      </c>
       <c r="I34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J34" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K34" s="3">
+        <v>33</v>
+      </c>
+      <c r="J34" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K34" s="4">
         <v>14.00</v>
       </c>
-      <c r="L34" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M34" s="3">
+      <c r="L34" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M34" s="4">
         <v>14.00</v>
       </c>
       <c r="N34">
@@ -1437,27 +1623,33 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F35">
         <v>29</v>
       </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>19052149</v>
+      </c>
       <c r="I35" t="s">
-        <v>38</v>
-      </c>
-      <c r="J35" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K35" s="3">
+        <v>40</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K35" s="4">
         <v>125.00</v>
       </c>
-      <c r="L35" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M35" s="3">
+      <c r="L35" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M35" s="4">
         <v>125.00</v>
       </c>
       <c r="N35">
@@ -1475,27 +1667,33 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E36" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F36">
         <v>30</v>
       </c>
+      <c r="G36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" t="s">
+        <v>24</v>
+      </c>
       <c r="I36" t="s">
-        <v>31</v>
-      </c>
-      <c r="J36" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="K36" s="3">
+        <v>33</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="K36" s="4">
         <v>123.00</v>
       </c>
-      <c r="L36" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="M36" s="3">
+      <c r="L36" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="M36" s="4">
         <v>123.00</v>
       </c>
       <c r="N36">
@@ -1513,27 +1711,33 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F37">
         <v>31</v>
       </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>32972358</v>
+      </c>
       <c r="I37" t="s">
-        <v>39</v>
-      </c>
-      <c r="J37" s="3">
+        <v>41</v>
+      </c>
+      <c r="J37" s="4">
         <v>41.53</v>
       </c>
-      <c r="K37" s="3">
-        <v>0.00</v>
-      </c>
-      <c r="L37" s="3">
+      <c r="K37" s="4">
+        <v>0.00</v>
+      </c>
+      <c r="L37" s="4">
         <v>7.47</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M37" s="4">
         <v>49.00</v>
       </c>
       <c r="N37">
@@ -1551,27 +1755,33 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F38">
         <v>32</v>
       </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>32850899</v>
+      </c>
       <c r="I38" t="s">
-        <v>40</v>
-      </c>
-      <c r="J38" s="3">
+        <v>42</v>
+      </c>
+      <c r="J38" s="4">
         <v>21.19</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="4">
         <v>90.00</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="4">
         <v>3.81</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M38" s="4">
         <v>115.00</v>
       </c>
       <c r="N38">
@@ -1579,17 +1789,17 @@
       </c>
     </row>
     <row r="39">
-      <c r="J39" s="3">
+      <c r="J39" s="4">
         <v>323.73</v>
       </c>
-      <c r="K39" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="L39" s="3">
+      <c r="K39" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="L39" s="4">
         <v>58.27</v>
       </c>
-      <c r="M39" t="s" s="4">
-        <v>42</v>
+      <c r="M39" t="s" s="3">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>